<commit_message>
Update compta sgeg le poireau
</commit_message>
<xml_diff>
--- a/COMPTA/Compta.xlsx
+++ b/COMPTA/Compta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bacs/Documents (non iCloud)/HujaTech/COMPTA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BE50B7-644D-FB4D-88C8-E12536A3A3AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD150F4-E392-0E4C-9D54-2D1473E27ECD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="460" windowWidth="24180" windowHeight="14520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="24180" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gérer mon argent" sheetId="1" r:id="rId1"/>
@@ -4755,13 +4755,13 @@
                 <c:formatCode>#,##0.00\ "€"</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6500</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>112.71000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>464.44</c:v>
+                  <c:v>264.44</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>55.59</c:v>
@@ -6903,8 +6903,8 @@
   </sheetPr>
   <dimension ref="B1:O34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="28.5" customHeight="1"/>
@@ -7089,7 +7089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:T39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -7993,8 +7993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="A10" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9012,7 +9012,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="102" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9055,10 +9055,10 @@
       </c>
       <c r="C3" s="43">
         <f>Revenu5[[#This Row],[Avant Remboursement]]-Revenu5[[#This Row],[Remboursement]]</f>
-        <v>6500</v>
+        <v>6000</v>
       </c>
       <c r="D3" s="15">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E3" s="10">
         <v>7000</v>
@@ -9093,9 +9093,11 @@
       </c>
       <c r="C5" s="43">
         <f>Revenu5[[#This Row],[Avant Remboursement]]-Revenu5[[#This Row],[Remboursement]]</f>
-        <v>464.44</v>
-      </c>
-      <c r="D5" s="15"/>
+        <v>264.44</v>
+      </c>
+      <c r="D5" s="15">
+        <v>200</v>
+      </c>
       <c r="E5" s="10">
         <f>Sortie!K8</f>
         <v>464.44</v>

</xml_diff>